<commit_message>
all working tables. at least hardcoded lastmile. but we are ready for calculations
</commit_message>
<xml_diff>
--- a/dataDir/models/Psku.xlsx
+++ b/dataDir/models/Psku.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -262,18 +265,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -281,43 +287,59 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="3">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -344,22 +366,82 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -371,149 +453,185 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -541,7 +659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -555,7 +673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -569,7 +687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -583,7 +701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -597,7 +715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -611,7 +729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -625,7 +743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -639,7 +757,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -653,7 +771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -667,7 +785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -681,7 +799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -695,7 +813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -709,7 +827,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -723,7 +841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -737,7 +855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -751,7 +869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
@@ -765,7 +883,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -779,7 +897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -793,7 +911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -807,7 +925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
@@ -821,7 +939,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
       <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
@@ -835,7 +953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
       <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
@@ -849,7 +967,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
@@ -863,7 +981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
       <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
@@ -877,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
       <c r="A27" s="1" t="s">
         <v>62</v>
       </c>
@@ -891,7 +1009,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
       <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
@@ -905,7 +1023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
@@ -919,7 +1037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="1" t="s">
         <v>68</v>
       </c>
@@ -933,7 +1051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
@@ -947,7 +1065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -961,7 +1079,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -975,7 +1093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -989,7 +1107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="1" t="s">
         <v>78</v>
       </c>
@@ -1003,7 +1121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
@@ -1018,6 +1136,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change in download btn
</commit_message>
<xml_diff>
--- a/dataDir/models/Psku.xlsx
+++ b/dataDir/models/Psku.xlsx
@@ -1,15 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
-  </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -265,21 +262,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -287,59 +281,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -366,82 +344,22 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="1155CC"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="1155CC"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,185 +371,149 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
-            </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-  </cols>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -659,7 +541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,7 +555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -687,7 +569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -701,7 +583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -715,7 +597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -729,7 +611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -743,7 +625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -757,7 +639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -771,7 +653,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -785,7 +667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -799,7 +681,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -813,7 +695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -827,7 +709,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -841,7 +723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -855,7 +737,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -869,7 +751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
@@ -883,7 +765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -897,7 +779,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -911,7 +793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -925,7 +807,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
@@ -939,7 +821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
@@ -953,7 +835,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
@@ -967,7 +849,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
@@ -981,7 +863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
@@ -995,7 +877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>62</v>
       </c>
@@ -1009,7 +891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
@@ -1023,7 +905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
@@ -1037,7 +919,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>68</v>
       </c>
@@ -1051,7 +933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
@@ -1065,7 +947,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -1079,7 +961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row r="33">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -1093,7 +975,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row r="34">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -1107,7 +989,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>78</v>
       </c>
@@ -1121,7 +1003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row r="36">
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
@@ -1136,6 +1018,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>